<commit_message>
From HackerEarth Sum of first N natural numbers problem solved
</commit_message>
<xml_diff>
--- a/NUMBERS_AND_MATH.xlsx
+++ b/NUMBERS_AND_MATH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Check if a number is palindrome or not</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Program to find roots of a Quadratic Equation</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Logic done</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,82 +476,109 @@
     <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -647,6 +680,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
From GFG Sum of GP solved
</commit_message>
<xml_diff>
--- a/NUMBERS_AND_MATH.xlsx
+++ b/NUMBERS_AND_MATH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Check if a number is palindrome or not</t>
   </si>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +551,9 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>